<commit_message>
feat: implemented Page Factory in InputPage
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E016F2D0-4D94-487E-965F-9763318A6173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB201AA4-A46D-4FFF-808F-933DAC161F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="33">
   <si>
     <t>From</t>
   </si>
@@ -81,12 +81,6 @@
     <t>https://erail.in/</t>
   </si>
   <si>
-    <t>Pun</t>
-  </si>
-  <si>
-    <t>Hyd</t>
-  </si>
-  <si>
     <t>Sleeper</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>24-Jun-25 Tue</t>
-  </si>
-  <si>
     <t>12702</t>
   </si>
   <si>
@@ -127,13 +118,33 @@
   </si>
   <si>
     <t>25-Jun-25 Wed</t>
+  </si>
+  <si>
+    <t>Gay</t>
+  </si>
+  <si>
+    <t>GAYA</t>
+  </si>
+  <si>
+    <t>Kol</t>
+  </si>
+  <si>
+    <t>KOAA</t>
+  </si>
+  <si>
+    <t>13152</t>
+  </si>
+  <si>
+    <t>KOLKATA EXPRESS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,17 +187,17 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -204,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,49 +238,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -605,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2210D17-C285-4D9E-A919-49370835DA19}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -640,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
@@ -648,36 +748,45 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f ca="1">TEXT(TODAY()+4, "dd-mmm-yy ddd")</f>
+        <v>25-Jun-25 Wed</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
-        <f ca="1">TODAY()+4</f>
-        <v>45832</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>16</v>
-      </c>
       <c r="F2" t="s" s="0">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -689,7 +798,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -725,8 +834,8 @@
       <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="46" t="s">
-        <v>21</v>
+      <c r="D2" s="135" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -739,8 +848,8 @@
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="47" t="s">
-        <v>21</v>
+      <c r="D3" s="136" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,13 +857,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="D4" s="137" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -762,28 +871,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="138" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B6" s="11" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd-mmm-yy ddd")</f>
-        <v>24-Jun-25 Tue</v>
+        <v>25-Jun-25 Wed</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D6" s="139" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat: Page Factory in Output
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="33">
   <si>
     <t>From</t>
   </si>
@@ -215,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -360,6 +360,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
@@ -834,7 +844,7 @@
       <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="135" t="s">
+      <c r="D2" s="145" t="s">
         <v>19</v>
       </c>
     </row>
@@ -848,7 +858,7 @@
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="146" t="s">
         <v>19</v>
       </c>
     </row>
@@ -862,7 +872,7 @@
       <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="137" t="s">
+      <c r="D4" s="147" t="s">
         <v>19</v>
       </c>
     </row>
@@ -876,7 +886,7 @@
       <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="138" t="s">
+      <c r="D5" s="148" t="s">
         <v>19</v>
       </c>
     </row>
@@ -891,7 +901,7 @@
       <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="139" t="s">
+      <c r="D6" s="149" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Modification in day input logic\
Number of Days input from Excel
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB201AA4-A46D-4FFF-808F-933DAC161F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7347E34A-34FC-4550-9377-3D9F5D90E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>From</t>
   </si>
@@ -87,33 +87,18 @@
     <t>Handicaped</t>
   </si>
   <si>
-    <t>HYB</t>
-  </si>
-  <si>
-    <t>PUNE</t>
-  </si>
-  <si>
     <t>Train Number</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>12702</t>
-  </si>
-  <si>
-    <t>HUSSAINSAGAR SF</t>
-  </si>
-  <si>
     <t>22731</t>
   </si>
   <si>
     <t>MUMBAI SF EXP</t>
   </si>
   <si>
-    <t xml:space="preserve"> Date</t>
-  </si>
-  <si>
     <t>FAIL</t>
   </si>
   <si>
@@ -136,6 +121,12 @@
   </si>
   <si>
     <t>KOLKATA EXPRESS</t>
+  </si>
+  <si>
+    <t>After Days</t>
+  </si>
+  <si>
+    <t>27-Jun-25 Fri</t>
   </si>
 </sst>
 </file>
@@ -215,12 +206,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -242,134 +232,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
@@ -717,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2210D17-C285-4D9E-A919-49370835DA19}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,38 +596,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">TEXT(TODAY()+4, "dd-mmm-yy ddd")</f>
-        <v>25-Jun-25 Wed</v>
+        <v>22</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0">
+        <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -774,18 +635,18 @@
         <v>14</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F3" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -807,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD26C9AB-AB7F-476E-83E1-568619EA48D3}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -827,7 +688,7 @@
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -835,78 +696,78 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="145" t="s">
-        <v>19</v>
+      <c r="D2" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="146" t="s">
-        <v>19</v>
+      <c r="D3" s="17" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="147" t="s">
-        <v>19</v>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="148" t="s">
-        <v>19</v>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="10" t="str">
         <f ca="1">TEXT(TODAY()+4, "dd-mmm-yy ddd")</f>
         <v>25-Jun-25 Wed</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="149" t="s">
-        <v>25</v>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
chore: Javadoc for TestMain
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7347E34A-34FC-4550-9377-3D9F5D90E5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145CF498-62E3-4359-8435-3EEF01B895E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>From</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>25-Jun-25 Wed</t>
   </si>
   <si>
     <t>Gay</t>
@@ -579,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2210D17-C285-4D9E-A919-49370835DA19}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -620,10 +617,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0">
         <v>6</v>
@@ -635,10 +632,10 @@
         <v>14</v>
       </c>
       <c r="F2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>26</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -668,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD26C9AB-AB7F-476E-83E1-568619EA48D3}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -728,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>17</v>
@@ -742,10 +739,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>17</v>
@@ -756,11 +753,11 @@
         <v>2</v>
       </c>
       <c r="B6" s="10" t="str">
-        <f ca="1">TEXT(TODAY()+4, "dd-mmm-yy ddd")</f>
-        <v>25-Jun-25 Wed</v>
+        <f ca="1">TEXT(TODAY()+SearchData!C2, "dd-mmm-yy ddd")</f>
+        <v>27-Jun-25 Fri</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
feat: writing train no and name in excel
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145CF498-62E3-4359-8435-3EEF01B895E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFF5E52-3832-4864-A4D4-66B830C9B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>From</t>
   </si>
@@ -90,40 +90,34 @@
     <t>Train Number</t>
   </si>
   <si>
+    <t>After Days</t>
+  </si>
+  <si>
+    <t>Coimb</t>
+  </si>
+  <si>
+    <t>CBE</t>
+  </si>
+  <si>
+    <t>Shali</t>
+  </si>
+  <si>
+    <t>SHM</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>22731</t>
-  </si>
-  <si>
-    <t>MUMBAI SF EXP</t>
+    <t>13-Jul-25 Sun</t>
+  </si>
+  <si>
+    <t>22641</t>
+  </si>
+  <si>
+    <t>SHALIMAR SF EXP</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Gay</t>
-  </si>
-  <si>
-    <t>GAYA</t>
-  </si>
-  <si>
-    <t>Kol</t>
-  </si>
-  <si>
-    <t>KOAA</t>
-  </si>
-  <si>
-    <t>13152</t>
-  </si>
-  <si>
-    <t>KOLKATA EXPRESS</t>
-  </si>
-  <si>
-    <t>After Days</t>
-  </si>
-  <si>
-    <t>27-Jun-25 Fri</t>
   </si>
 </sst>
 </file>
@@ -175,17 +169,17 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="none">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -203,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,27 +212,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,7 +570,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -617,13 +610,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C2" s="0">
         <v>21</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C2" s="0">
-        <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -632,18 +625,10 @@
         <v>14</v>
       </c>
       <c r="F2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>25</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -663,7 +648,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD26C9AB-AB7F-476E-83E1-568619EA48D3}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -672,8 +657,8 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="14.6328125"/>
-    <col min="2" max="2" customWidth="true" width="20.54296875"/>
-    <col min="3" max="3" customWidth="true" width="16.90625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="59.08984375"/>
+    <col min="3" max="3" customWidth="true" width="59.54296875"/>
     <col min="4" max="4" customWidth="true" width="17.0"/>
     <col min="5" max="16384" hidden="true" width="8.7265625"/>
   </cols>
@@ -685,7 +670,7 @@
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -702,8 +687,8 @@
       <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>17</v>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -716,8 +701,8 @@
       <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>17</v>
+      <c r="D3" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -725,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -739,33 +724,42 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B6" s="7" t="str">
         <f ca="1">TEXT(TODAY()+SearchData!C2, "dd-mmm-yy ddd")</f>
-        <v>27-Jun-25 Fri</v>
+        <v>13-Jul-25 Sun</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="C7" s="3"/>
     </row>
+    <row r="17" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="18" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="19" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="20" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="21" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="22" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="23" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="24" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="25" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{DDA58F1D-300E-4C8B-B825-97010CBADDF4}"/>

</xml_diff>

<commit_message>
fix(developer-ui): filter out unwanted dates from last month
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFF5E52-3832-4864-A4D4-66B830C9B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FFC294-F328-4D93-8AD4-E8B0E961754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>From</t>
   </si>
@@ -108,16 +108,25 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>13-Jul-25 Sun</t>
+    <t>14-Jul-25 Mon</t>
+  </si>
+  <si>
+    <t>12659</t>
+  </si>
+  <si>
+    <t>GURUDEV SF EXP</t>
+  </si>
+  <si>
+    <t>05-Oct-25 Sun</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
   <si>
     <t>22641</t>
   </si>
   <si>
     <t>SHALIMAR SF EXP</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -570,7 +579,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="0">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
@@ -625,10 +634,10 @@
         <v>14</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -648,7 +657,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD26C9AB-AB7F-476E-83E1-568619EA48D3}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -739,13 +748,13 @@
       </c>
       <c r="B6" s="7" t="str">
         <f ca="1">TEXT(TODAY()+SearchData!C2, "dd-mmm-yy ddd")</f>
-        <v>13-Jul-25 Sun</v>
+        <v>05-Oct-25 Sun</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
@@ -760,6 +769,12 @@
     <row r="23" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="24" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="25" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="26" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="27" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="28" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="29" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="30" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="31" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{DDA58F1D-300E-4C8B-B825-97010CBADDF4}"/>

</xml_diff>

<commit_message>
feat: Added SSL Acceptance in Options
</commit_message>
<xml_diff>
--- a/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
+++ b/src/test/java/com/selenium/test/data/TrainSearchData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Automation\workspace\TrainSearchAutomation\src\test\java\com\selenium\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FFC294-F328-4D93-8AD4-E8B0E961754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5833C4C6-1F87-4153-BD33-BFFB2F9354CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9161C4F-4C8C-4984-A117-FA49C1C684A3}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>From</t>
   </si>
@@ -105,28 +105,13 @@
     <t>SHM</t>
   </si>
   <si>
+    <t>11-Sep-25 Thu</t>
+  </si>
+  <si>
+    <t>Copy  &amp; Paste this date in Expected in string to see PASS</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>14-Jul-25 Mon</t>
-  </si>
-  <si>
-    <t>12659</t>
-  </si>
-  <si>
-    <t>GURUDEV SF EXP</t>
-  </si>
-  <si>
-    <t>05-Oct-25 Sun</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>22641</t>
-  </si>
-  <si>
-    <t>SHALIMAR SF EXP</t>
   </si>
 </sst>
 </file>
@@ -153,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,7 +159,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -183,13 +169,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -206,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,23 +205,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2210D17-C285-4D9E-A919-49370835DA19}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,19 +610,13 @@
         <v>20</v>
       </c>
       <c r="C2" s="0">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -657,10 +636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD26C9AB-AB7F-476E-83E1-568619EA48D3}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -693,11 +672,11 @@
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>22</v>
+      <c r="D2" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -707,11 +686,11 @@
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>22</v>
+      <c r="D3" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -721,11 +700,11 @@
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>22</v>
+      <c r="D4" s="19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -735,46 +714,52 @@
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="str">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="str">
         <f ca="1">TEXT(TODAY()+SearchData!C2, "dd-mmm-yy ddd")</f>
-        <v>05-Oct-25 Sun</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="3"/>
-    </row>
-    <row r="17" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="18" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="19" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="20" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="21" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="22" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="23" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="24" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="25" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="26" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="27" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="28" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="29" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="30" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="31" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+        <v>11-Sep-25 Thu</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="34" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="35" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="36" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="37" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="38" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="39" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="40" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="41" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="42" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="43" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="44" customFormat="1" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{DDA58F1D-300E-4C8B-B825-97010CBADDF4}"/>

</xml_diff>